<commit_message>
code update - attempt 1
</commit_message>
<xml_diff>
--- a/AmazonFlipkartProject/TestData.xlsx
+++ b/AmazonFlipkartProject/TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D9805031-11EA-4DEA-B114-B87BF843D636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdoshi\Desktop\ZestMoneyAssignment\AmazonFlipkartProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4732C68-701A-4DA5-8FCE-1F11D05C9605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="17970" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M6"/>
 </workbook>
 </file>
 
@@ -29,9 +33,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>LoginTest001</t>
-  </si>
-  <si>
     <t>UserId</t>
   </si>
   <si>
@@ -141,6 +142,9 @@
   </si>
   <si>
     <t>12345!@</t>
+  </si>
+  <si>
+    <t>LoginTest</t>
   </si>
 </sst>
 </file>
@@ -547,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL13"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,495 +595,121 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="U1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AE1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="AL1" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-    </row>
-    <row r="4" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-    </row>
-    <row r="5" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-    </row>
-    <row r="6" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-    </row>
-    <row r="7" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-    </row>
-    <row r="8" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-    </row>
-    <row r="9" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-    </row>
-    <row r="10" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-    </row>
-    <row r="11" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-    </row>
-    <row r="12" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-    </row>
-    <row r="13" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>